<commit_message>
Finished exploratory data analysis of columns with no missing values and generated a summary report
</commit_message>
<xml_diff>
--- a/Data Cleaning and feature engineering report/statistics_columns_with_missing_values.xlsx
+++ b/Data Cleaning and feature engineering report/statistics_columns_with_missing_values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gangu\OneDrive\Desktop\Academics\Predictive model to classify profitable borrowers\Data Cleaning and feature engineering report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D061342B-1324-452D-9E0E-58375E0F2518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B362B8-5B4E-4E22-951F-995210F6F05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1589,6 +1589,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1599,9 +1602,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4872,12 +4872,12 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="52"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
       <c r="O1" s="68" t="s">
         <v>58</v>
       </c>
@@ -4896,10 +4896,10 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
       <c r="O2" s="85" t="s">
         <v>81</v>
       </c>
@@ -4985,7 +4985,7 @@
       <c r="L5" s="19">
         <v>8625</v>
       </c>
-      <c r="M5" s="86" t="s">
+      <c r="M5" s="87" t="s">
         <v>69</v>
       </c>
       <c r="O5" s="85"/>
@@ -5006,7 +5006,7 @@
       <c r="L6" s="19">
         <v>5440.2000000000098</v>
       </c>
-      <c r="M6" s="86"/>
+      <c r="M6" s="87"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
@@ -5043,7 +5043,7 @@
       <c r="L7" s="19">
         <v>5086.7999999999802</v>
       </c>
-      <c r="M7" s="86"/>
+      <c r="M7" s="87"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
@@ -5080,7 +5080,7 @@
       <c r="L8" s="19">
         <v>5017</v>
       </c>
-      <c r="M8" s="86"/>
+      <c r="M8" s="87"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -5117,7 +5117,7 @@
       <c r="L9" s="19">
         <v>5254</v>
       </c>
-      <c r="M9" s="86"/>
+      <c r="M9" s="87"/>
       <c r="O9" s="69" t="s">
         <v>59</v>
       </c>
@@ -5156,7 +5156,7 @@
       <c r="L10" s="19">
         <v>5884</v>
       </c>
-      <c r="M10" s="86"/>
+      <c r="M10" s="87"/>
       <c r="O10" s="80" t="s">
         <v>157</v>
       </c>
@@ -5195,14 +5195,14 @@
       <c r="L11" s="19">
         <v>6893.6999999999498</v>
       </c>
-      <c r="M11" s="86"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="90"/>
+      <c r="M11" s="87"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="T11" s="86"/>
+      <c r="U11" s="86"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -5232,14 +5232,14 @@
       <c r="L12" s="19">
         <v>8751.3000000000393</v>
       </c>
-      <c r="M12" s="86"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="90"/>
-      <c r="U12" s="90"/>
+      <c r="M12" s="87"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
+      <c r="T12" s="86"/>
+      <c r="U12" s="86"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -5269,14 +5269,14 @@
       <c r="L13" s="19">
         <v>11991</v>
       </c>
-      <c r="M13" s="86"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="90"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
+      <c r="M13" s="87"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="86"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -5306,7 +5306,7 @@
       <c r="L14" s="19">
         <v>17288</v>
       </c>
-      <c r="M14" s="86"/>
+      <c r="M14" s="87"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -5336,7 +5336,7 @@
       <c r="L15" s="15">
         <v>23130</v>
       </c>
-      <c r="M15" s="87" t="s">
+      <c r="M15" s="88" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5368,7 +5368,7 @@
       <c r="L16" s="15">
         <v>26472.199999999899</v>
       </c>
-      <c r="M16" s="87"/>
+      <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -5398,7 +5398,7 @@
       <c r="L17" s="15">
         <v>26124.799999999999</v>
       </c>
-      <c r="M17" s="87"/>
+      <c r="M17" s="88"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -5428,7 +5428,7 @@
       <c r="L18" s="15">
         <v>26162</v>
       </c>
-      <c r="M18" s="87"/>
+      <c r="M18" s="88"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -5458,7 +5458,7 @@
       <c r="L19" s="15">
         <v>28595</v>
       </c>
-      <c r="M19" s="87"/>
+      <c r="M19" s="88"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J20" s="14">
@@ -5470,7 +5470,7 @@
       <c r="L20" s="15">
         <v>33341.599999999999</v>
       </c>
-      <c r="M20" s="87"/>
+      <c r="M20" s="88"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J21" s="14">
@@ -5482,7 +5482,7 @@
       <c r="L21" s="15">
         <v>40955.3999999999</v>
       </c>
-      <c r="M21" s="87"/>
+      <c r="M21" s="88"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J22" s="14">
@@ -5494,7 +5494,7 @@
       <c r="L22" s="15">
         <v>55353</v>
       </c>
-      <c r="M22" s="87"/>
+      <c r="M22" s="88"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J23" s="16">
@@ -5506,7 +5506,7 @@
       <c r="L23" s="17">
         <v>93108</v>
       </c>
-      <c r="M23" s="88" t="s">
+      <c r="M23" s="89" t="s">
         <v>72</v>
       </c>
     </row>
@@ -5520,7 +5520,7 @@
       <c r="L24" s="17">
         <v>29321.4399999999</v>
       </c>
-      <c r="M24" s="88"/>
+      <c r="M24" s="89"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J25" s="16">
@@ -5532,7 +5532,7 @@
       <c r="L25" s="17">
         <v>18197.560000000001</v>
       </c>
-      <c r="M25" s="88"/>
+      <c r="M25" s="89"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J26" s="16">
@@ -5544,7 +5544,7 @@
       <c r="L26" s="17">
         <v>21789</v>
       </c>
-      <c r="M26" s="88"/>
+      <c r="M26" s="89"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J27" s="16">
@@ -5556,7 +5556,7 @@
       <c r="L27" s="17">
         <v>26955.8999999999</v>
       </c>
-      <c r="M27" s="88"/>
+      <c r="M27" s="89"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J28" s="16">
@@ -5568,7 +5568,7 @@
       <c r="L28" s="17">
         <v>33622.939999997601</v>
       </c>
-      <c r="M28" s="88"/>
+      <c r="M28" s="89"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J29" s="16">
@@ -5580,7 +5580,7 @@
       <c r="L29" s="17">
         <v>45328.0500000026</v>
       </c>
-      <c r="M29" s="88"/>
+      <c r="M29" s="89"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J30" s="16">
@@ -5592,7 +5592,7 @@
       <c r="L30" s="17">
         <v>65600.709999998493</v>
       </c>
-      <c r="M30" s="88"/>
+      <c r="M30" s="89"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J31" s="16">
@@ -5604,7 +5604,7 @@
       <c r="L31" s="17">
         <v>131934.640000004</v>
       </c>
-      <c r="M31" s="88"/>
+      <c r="M31" s="89"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J32" s="20">
@@ -5622,6 +5622,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="M15:M22"/>
+    <mergeCell ref="M23:M31"/>
+    <mergeCell ref="J1:M2"/>
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="O2:U7"/>
     <mergeCell ref="O9:U9"/>
@@ -5629,9 +5632,6 @@
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="B1:G5"/>
     <mergeCell ref="M5:M14"/>
-    <mergeCell ref="M15:M22"/>
-    <mergeCell ref="M23:M31"/>
-    <mergeCell ref="J1:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6434,8 +6434,8 @@
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
       <c r="J2" s="98"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
       <c r="M2" s="99"/>
       <c r="O2" s="85" t="s">
         <v>80</v>
@@ -6521,7 +6521,7 @@
       <c r="L5" s="28">
         <v>1100</v>
       </c>
-      <c r="M5" s="86" t="s">
+      <c r="M5" s="87" t="s">
         <v>69</v>
       </c>
       <c r="O5" s="85"/>
@@ -6542,7 +6542,7 @@
       <c r="L6" s="28">
         <v>540</v>
       </c>
-      <c r="M6" s="86"/>
+      <c r="M6" s="87"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
@@ -6579,7 +6579,7 @@
       <c r="L7" s="28">
         <v>488</v>
       </c>
-      <c r="M7" s="86"/>
+      <c r="M7" s="87"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
@@ -6616,7 +6616,7 @@
       <c r="L8" s="28">
         <v>477</v>
       </c>
-      <c r="M8" s="86"/>
+      <c r="M8" s="87"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -6653,7 +6653,7 @@
       <c r="L9" s="28">
         <v>496</v>
       </c>
-      <c r="M9" s="86"/>
+      <c r="M9" s="87"/>
       <c r="O9" s="69" t="s">
         <v>59</v>
       </c>
@@ -6692,7 +6692,7 @@
       <c r="L10" s="28">
         <v>542</v>
       </c>
-      <c r="M10" s="86"/>
+      <c r="M10" s="87"/>
       <c r="O10" s="80" t="s">
         <v>159</v>
       </c>
@@ -6731,14 +6731,14 @@
       <c r="L11" s="28">
         <v>636</v>
       </c>
-      <c r="M11" s="86"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="90"/>
+      <c r="M11" s="87"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="T11" s="86"/>
+      <c r="U11" s="86"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -6768,14 +6768,14 @@
       <c r="L12" s="28">
         <v>779</v>
       </c>
-      <c r="M12" s="86"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="90"/>
-      <c r="U12" s="90"/>
+      <c r="M12" s="87"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
+      <c r="T12" s="86"/>
+      <c r="U12" s="86"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -6805,14 +6805,14 @@
       <c r="L13" s="28">
         <v>999</v>
       </c>
-      <c r="M13" s="86"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="90"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
+      <c r="M13" s="87"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="86"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -6842,7 +6842,7 @@
       <c r="L14" s="30">
         <v>1350</v>
       </c>
-      <c r="M14" s="87" t="s">
+      <c r="M14" s="88" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6874,7 +6874,7 @@
       <c r="L15" s="30">
         <v>1738</v>
       </c>
-      <c r="M15" s="87"/>
+      <c r="M15" s="88"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -6904,7 +6904,7 @@
       <c r="L16" s="30">
         <v>2054</v>
       </c>
-      <c r="M16" s="87"/>
+      <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -6934,7 +6934,7 @@
       <c r="L17" s="30">
         <v>2247</v>
       </c>
-      <c r="M17" s="87"/>
+      <c r="M17" s="88"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -6964,7 +6964,7 @@
       <c r="L18" s="30">
         <v>2471</v>
       </c>
-      <c r="M18" s="87"/>
+      <c r="M18" s="88"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -6994,7 +6994,7 @@
       <c r="L19" s="30">
         <v>2800</v>
       </c>
-      <c r="M19" s="87"/>
+      <c r="M19" s="88"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J20" s="29">
@@ -7006,7 +7006,7 @@
       <c r="L20" s="30">
         <v>3322</v>
       </c>
-      <c r="M20" s="87"/>
+      <c r="M20" s="88"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J21" s="29">
@@ -7018,7 +7018,7 @@
       <c r="L21" s="30">
         <v>4220</v>
       </c>
-      <c r="M21" s="87"/>
+      <c r="M21" s="88"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J22" s="29">
@@ -7030,7 +7030,7 @@
       <c r="L22" s="30">
         <v>5961</v>
       </c>
-      <c r="M22" s="87"/>
+      <c r="M22" s="88"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J23" s="31">
@@ -7042,7 +7042,7 @@
       <c r="L23" s="32">
         <v>10825</v>
       </c>
-      <c r="M23" s="88" t="s">
+      <c r="M23" s="89" t="s">
         <v>72</v>
       </c>
     </row>
@@ -7056,7 +7056,7 @@
       <c r="L24" s="32">
         <v>3665.6</v>
       </c>
-      <c r="M24" s="88"/>
+      <c r="M24" s="89"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J25" s="31">
@@ -7068,7 +7068,7 @@
       <c r="L25" s="32">
         <v>2284.8000000000002</v>
       </c>
-      <c r="M25" s="88"/>
+      <c r="M25" s="89"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J26" s="31">
@@ -7080,7 +7080,7 @@
       <c r="L26" s="32">
         <v>2706.8</v>
       </c>
-      <c r="M26" s="88"/>
+      <c r="M26" s="89"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J27" s="31">
@@ -7092,7 +7092,7 @@
       <c r="L27" s="32">
         <v>3319.8</v>
       </c>
-      <c r="M27" s="88"/>
+      <c r="M27" s="89"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J28" s="31">
@@ -7104,7 +7104,7 @@
       <c r="L28" s="32">
         <v>4232</v>
       </c>
-      <c r="M28" s="88"/>
+      <c r="M28" s="89"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J29" s="31">
@@ -7116,7 +7116,7 @@
       <c r="L29" s="32">
         <v>5699.8</v>
       </c>
-      <c r="M29" s="88"/>
+      <c r="M29" s="89"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J30" s="31">
@@ -7128,7 +7128,7 @@
       <c r="L30" s="32">
         <v>8573</v>
       </c>
-      <c r="M30" s="88"/>
+      <c r="M30" s="89"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J31" s="31">
@@ -7140,7 +7140,7 @@
       <c r="L31" s="32">
         <v>16627.2</v>
       </c>
-      <c r="M31" s="88"/>
+      <c r="M31" s="89"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J32" s="33">
@@ -7158,16 +7158,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="M14:M22"/>
+    <mergeCell ref="M23:M31"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="B1:G5"/>
+    <mergeCell ref="J1:M2"/>
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="O2:U7"/>
     <mergeCell ref="O9:U9"/>
     <mergeCell ref="O10:U13"/>
     <mergeCell ref="M5:M13"/>
-    <mergeCell ref="M14:M22"/>
-    <mergeCell ref="M23:M31"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="B1:G5"/>
-    <mergeCell ref="J1:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8146,9 +8146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889A2433-60D7-4D50-A2C2-8D0431AB97E1}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9917,15 +9915,15 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="49"/>
@@ -9935,13 +9933,13 @@
       <c r="E3" s="53"/>
       <c r="F3" s="53"/>
       <c r="G3" s="54"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="49"/>
@@ -12984,15 +12982,15 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="49"/>
@@ -13002,13 +13000,13 @@
       <c r="E3" s="53"/>
       <c r="F3" s="53"/>
       <c r="G3" s="54"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
     </row>
     <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="49"/>
@@ -17777,15 +17775,15 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="49"/>
@@ -17795,13 +17793,13 @@
       <c r="E3" s="53"/>
       <c r="F3" s="53"/>
       <c r="G3" s="54"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="49"/>
@@ -20562,12 +20560,12 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="52"/>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
       <c r="N1" s="68" t="s">
         <v>58</v>
       </c>
@@ -20586,10 +20584,10 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
       <c r="N2" s="85" t="s">
         <v>137</v>
       </c>
@@ -20673,7 +20671,7 @@
       <c r="K5" s="28">
         <v>6848</v>
       </c>
-      <c r="L5" s="86" t="s">
+      <c r="L5" s="87" t="s">
         <v>69</v>
       </c>
       <c r="N5" s="85"/>
@@ -20694,7 +20692,7 @@
       <c r="K6" s="28">
         <v>4038</v>
       </c>
-      <c r="L6" s="86"/>
+      <c r="L6" s="87"/>
       <c r="N6" s="85"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
@@ -20731,7 +20729,7 @@
       <c r="K7" s="28">
         <v>3517</v>
       </c>
-      <c r="L7" s="86"/>
+      <c r="L7" s="87"/>
       <c r="N7" s="85"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
@@ -20768,7 +20766,7 @@
       <c r="K8" s="28">
         <v>3311</v>
       </c>
-      <c r="L8" s="86"/>
+      <c r="L8" s="87"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -20805,7 +20803,7 @@
       <c r="K9" s="28">
         <v>3172</v>
       </c>
-      <c r="L9" s="86"/>
+      <c r="L9" s="87"/>
       <c r="N9" s="69" t="s">
         <v>59</v>
       </c>
@@ -20844,7 +20842,7 @@
       <c r="K10" s="28">
         <v>3106</v>
       </c>
-      <c r="L10" s="86"/>
+      <c r="L10" s="87"/>
       <c r="N10" s="79" t="s">
         <v>164</v>
       </c>
@@ -20883,13 +20881,13 @@
       <c r="K11" s="28">
         <v>3135</v>
       </c>
-      <c r="L11" s="86"/>
+      <c r="L11" s="87"/>
       <c r="N11" s="100"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
       <c r="T11" s="101"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -20920,13 +20918,13 @@
       <c r="K12" s="28">
         <v>3222</v>
       </c>
-      <c r="L12" s="86"/>
+      <c r="L12" s="87"/>
       <c r="N12" s="100"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
       <c r="T12" s="101"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -20957,7 +20955,7 @@
       <c r="K13" s="28">
         <v>3372</v>
       </c>
-      <c r="L13" s="86"/>
+      <c r="L13" s="87"/>
       <c r="N13" s="82"/>
       <c r="O13" s="83"/>
       <c r="P13" s="83"/>
@@ -20994,7 +20992,7 @@
       <c r="K14" s="28">
         <v>3575</v>
       </c>
-      <c r="L14" s="86"/>
+      <c r="L14" s="87"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -21024,7 +21022,7 @@
       <c r="K15" s="28">
         <v>3835</v>
       </c>
-      <c r="L15" s="86"/>
+      <c r="L15" s="87"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -21054,7 +21052,7 @@
       <c r="K16" s="28">
         <v>4262</v>
       </c>
-      <c r="L16" s="86"/>
+      <c r="L16" s="87"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -21427,12 +21425,12 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="52"/>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
       <c r="N1" s="68" t="s">
         <v>58</v>
       </c>
@@ -21451,10 +21449,10 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
       <c r="N2" s="85" t="s">
         <v>138</v>
       </c>
@@ -21538,7 +21536,7 @@
       <c r="K5" s="28">
         <v>2300</v>
       </c>
-      <c r="L5" s="86" t="s">
+      <c r="L5" s="87" t="s">
         <v>69</v>
       </c>
       <c r="N5" s="85"/>
@@ -21559,7 +21557,7 @@
       <c r="K6" s="28">
         <v>1600</v>
       </c>
-      <c r="L6" s="86"/>
+      <c r="L6" s="87"/>
       <c r="N6" s="85"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
@@ -21596,7 +21594,7 @@
       <c r="K7" s="28">
         <v>1300</v>
       </c>
-      <c r="L7" s="86"/>
+      <c r="L7" s="87"/>
       <c r="N7" s="85"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
@@ -21633,7 +21631,7 @@
       <c r="K8" s="28">
         <v>1300</v>
       </c>
-      <c r="L8" s="86"/>
+      <c r="L8" s="87"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -21670,7 +21668,7 @@
       <c r="K9" s="28">
         <v>1300</v>
       </c>
-      <c r="L9" s="86"/>
+      <c r="L9" s="87"/>
       <c r="N9" s="69" t="s">
         <v>59</v>
       </c>
@@ -21709,7 +21707,7 @@
       <c r="K10" s="28">
         <v>1200</v>
       </c>
-      <c r="L10" s="86"/>
+      <c r="L10" s="87"/>
       <c r="N10" s="79" t="s">
         <v>165</v>
       </c>
@@ -21748,13 +21746,13 @@
       <c r="K11" s="28">
         <v>1400</v>
       </c>
-      <c r="L11" s="86"/>
+      <c r="L11" s="87"/>
       <c r="N11" s="100"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
       <c r="T11" s="101"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -21785,13 +21783,13 @@
       <c r="K12" s="28">
         <v>1400</v>
       </c>
-      <c r="L12" s="86"/>
+      <c r="L12" s="87"/>
       <c r="N12" s="100"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
       <c r="T12" s="101"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -21822,7 +21820,7 @@
       <c r="K13" s="28">
         <v>1600</v>
       </c>
-      <c r="L13" s="86"/>
+      <c r="L13" s="87"/>
       <c r="N13" s="82"/>
       <c r="O13" s="83"/>
       <c r="P13" s="83"/>
@@ -21859,7 +21857,7 @@
       <c r="K14" s="28">
         <v>1700</v>
       </c>
-      <c r="L14" s="86"/>
+      <c r="L14" s="87"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -21889,7 +21887,7 @@
       <c r="K15" s="28">
         <v>1900</v>
       </c>
-      <c r="L15" s="86"/>
+      <c r="L15" s="87"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -21919,7 +21917,7 @@
       <c r="K16" s="28">
         <v>2100</v>
       </c>
-      <c r="L16" s="86"/>
+      <c r="L16" s="87"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -22292,12 +22290,12 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="52"/>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
       <c r="N1" s="68" t="s">
         <v>58</v>
       </c>
@@ -22316,10 +22314,10 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
       <c r="N2" s="85" t="s">
         <v>139</v>
       </c>
@@ -22403,7 +22401,7 @@
       <c r="K5" s="28">
         <v>0</v>
       </c>
-      <c r="L5" s="86" t="s">
+      <c r="L5" s="87" t="s">
         <v>69</v>
       </c>
       <c r="N5" s="85"/>
@@ -22424,7 +22422,7 @@
       <c r="K6" s="28">
         <v>0</v>
       </c>
-      <c r="L6" s="86"/>
+      <c r="L6" s="87"/>
       <c r="N6" s="85"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
@@ -22461,7 +22459,7 @@
       <c r="K7" s="28">
         <v>6000</v>
       </c>
-      <c r="L7" s="86"/>
+      <c r="L7" s="87"/>
       <c r="N7" s="85"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
@@ -22498,7 +22496,7 @@
       <c r="K8" s="28">
         <v>4530</v>
       </c>
-      <c r="L8" s="86"/>
+      <c r="L8" s="87"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -22535,7 +22533,7 @@
       <c r="K9" s="28">
         <v>4208</v>
       </c>
-      <c r="L9" s="86"/>
+      <c r="L9" s="87"/>
       <c r="N9" s="69" t="s">
         <v>59</v>
       </c>
@@ -22574,7 +22572,7 @@
       <c r="K10" s="28">
         <v>3355</v>
       </c>
-      <c r="L10" s="86"/>
+      <c r="L10" s="87"/>
       <c r="N10" s="79" t="s">
         <v>165</v>
       </c>
@@ -22613,13 +22611,13 @@
       <c r="K11" s="28">
         <v>3331</v>
       </c>
-      <c r="L11" s="86"/>
+      <c r="L11" s="87"/>
       <c r="N11" s="100"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
       <c r="T11" s="101"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -22650,13 +22648,13 @@
       <c r="K12" s="28">
         <v>3384</v>
       </c>
-      <c r="L12" s="86"/>
+      <c r="L12" s="87"/>
       <c r="N12" s="100"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
       <c r="T12" s="101"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -22687,7 +22685,7 @@
       <c r="K13" s="28">
         <v>3304</v>
       </c>
-      <c r="L13" s="86"/>
+      <c r="L13" s="87"/>
       <c r="N13" s="82"/>
       <c r="O13" s="83"/>
       <c r="P13" s="83"/>
@@ -22724,7 +22722,7 @@
       <c r="K14" s="28">
         <v>3569</v>
       </c>
-      <c r="L14" s="86"/>
+      <c r="L14" s="87"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -22754,7 +22752,7 @@
       <c r="K15" s="28">
         <v>3862</v>
       </c>
-      <c r="L15" s="86"/>
+      <c r="L15" s="87"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -22784,7 +22782,7 @@
       <c r="K16" s="28">
         <v>4289</v>
       </c>
-      <c r="L16" s="86"/>
+      <c r="L16" s="87"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -22814,7 +22812,7 @@
       <c r="K17" s="28">
         <v>4762</v>
       </c>
-      <c r="L17" s="86"/>
+      <c r="L17" s="87"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -22844,7 +22842,7 @@
       <c r="K18" s="30">
         <v>5503</v>
       </c>
-      <c r="L18" s="87" t="s">
+      <c r="L18" s="88" t="s">
         <v>71</v>
       </c>
     </row>
@@ -22876,7 +22874,7 @@
       <c r="K19" s="30">
         <v>6538</v>
       </c>
-      <c r="L19" s="87"/>
+      <c r="L19" s="88"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I20" s="29">
@@ -22888,7 +22886,7 @@
       <c r="K20" s="30">
         <v>8079.6</v>
       </c>
-      <c r="L20" s="87"/>
+      <c r="L20" s="88"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="37"/>
@@ -22901,7 +22899,7 @@
       <c r="K21" s="30">
         <v>10567.4</v>
       </c>
-      <c r="L21" s="87"/>
+      <c r="L21" s="88"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
@@ -22914,7 +22912,7 @@
       <c r="K22" s="30">
         <v>15410.8</v>
       </c>
-      <c r="L22" s="87"/>
+      <c r="L22" s="88"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="37"/>
@@ -22927,7 +22925,7 @@
       <c r="K23" s="32">
         <v>29416.2</v>
       </c>
-      <c r="L23" s="88" t="s">
+      <c r="L23" s="89" t="s">
         <v>72</v>
       </c>
     </row>
@@ -22942,7 +22940,7 @@
       <c r="K24" s="32">
         <v>10128.719999999999</v>
       </c>
-      <c r="L24" s="88"/>
+      <c r="L24" s="89"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
@@ -22955,7 +22953,7 @@
       <c r="K25" s="32">
         <v>6325.91</v>
       </c>
-      <c r="L25" s="88"/>
+      <c r="L25" s="89"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
@@ -22968,7 +22966,7 @@
       <c r="K26" s="32">
         <v>7655.91</v>
       </c>
-      <c r="L26" s="88"/>
+      <c r="L26" s="89"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
@@ -22981,7 +22979,7 @@
       <c r="K27" s="32">
         <v>9246.91</v>
       </c>
-      <c r="L27" s="88"/>
+      <c r="L27" s="89"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
@@ -22994,7 +22992,7 @@
       <c r="K28" s="32">
         <v>11998.91</v>
       </c>
-      <c r="L28" s="88"/>
+      <c r="L28" s="89"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
@@ -23007,7 +23005,7 @@
       <c r="K29" s="32">
         <v>15583.64</v>
       </c>
-      <c r="L29" s="88"/>
+      <c r="L29" s="89"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
@@ -23020,7 +23018,7 @@
       <c r="K30" s="32">
         <v>22602.26</v>
       </c>
-      <c r="L30" s="88"/>
+      <c r="L30" s="89"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
@@ -23033,7 +23031,7 @@
       <c r="K31" s="32">
         <v>42227.73</v>
       </c>
-      <c r="L31" s="88"/>
+      <c r="L31" s="89"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>

</xml_diff>